<commit_message>
Review is completed by Furkan Kara
</commit_message>
<xml_diff>
--- a/Task3/SW-TEAM-NEPTUNE/Ömer/[e.yigit][tractionControlManager][27.03.2025]_ImplementationReview.xlsx
+++ b/Task3/SW-TEAM-NEPTUNE/Ömer/[e.yigit][tractionControlManager][27.03.2025]_ImplementationReview.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MONSTER\OneDrive\Masaüstü\rewiev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furkan\EEM_TASK\Task3\SW-TEAM-NEPTUNE\Ömer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820DFB27-451B-4859-9FE1-AB44EE51AED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1D1F0-5148-4918-86F2-30C2F890CF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27684" yWindow="7992" windowWidth="23064" windowHeight="6120" xr2:uid="{54E6E97C-3F70-432C-B2C3-092D5DC5BF83}"/>
+    <workbookView xWindow="14976" yWindow="0" windowWidth="10263" windowHeight="13536" xr2:uid="{54E6E97C-3F70-432C-B2C3-092D5DC5BF83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
   <si>
     <t>Component Implementation Check list</t>
   </si>
@@ -128,13 +128,13 @@
     <t>Onaylanmıştır.</t>
   </si>
   <si>
-    <t>[Developer Name]</t>
-  </si>
-  <si>
     <t>[Architect Name]</t>
   </si>
   <si>
     <t>Erhan Can YİĞİT</t>
+  </si>
+  <si>
+    <t>Furkan Kara</t>
   </si>
 </sst>
 </file>
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -349,21 +349,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -482,7 +467,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -491,15 +476,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -878,11 +862,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B862DCFF-690B-4FC9-B9E6-BE6D2652C122}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="75.88671875" customWidth="1"/>
     <col min="2" max="2" width="18.109375" customWidth="1"/>
@@ -893,7 +877,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -905,28 +889,28 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="11" t="s">
         <v>25</v>
       </c>
     </row>
@@ -934,15 +918,17 @@
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1"/>
+      <c r="B3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D3" s="4"/>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>26</v>
       </c>
     </row>
@@ -950,15 +936,17 @@
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="1"/>
+      <c r="B4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="F4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -966,15 +954,17 @@
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" s="4"/>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>28</v>
       </c>
     </row>
@@ -982,15 +972,17 @@
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1"/>
+      <c r="B6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D6" s="4"/>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>29</v>
       </c>
     </row>
@@ -998,114 +990,134 @@
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="1"/>
+      <c r="B7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="1"/>
+      <c r="B8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1"/>
+      <c r="B9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1"/>
+      <c r="B10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="12" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="1"/>
+      <c r="B14" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="1"/>
+      <c r="B15" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>21</v>
+      </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
+      <c r="B16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:A2"/>
   </mergeCells>
-  <conditionalFormatting sqref="F4:F5">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F5">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>